<commit_message>
adjusted datatype on xlsx colums.
</commit_message>
<xml_diff>
--- a/input/rds_template.xlsx
+++ b/input/rds_template.xlsx
@@ -452,7 +452,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,6 +481,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -894,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1160,7 +1162,7 @@
     <row r="14" spans="1:10">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="3"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
@@ -1171,7 +1173,7 @@
     <row r="15" spans="1:10">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="3"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
@@ -1515,7 +1517,7 @@
     <row r="43" spans="1:10">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="3"/>
       <c r="G43" s="9">
         <v>23</v>
@@ -1527,7 +1529,7 @@
     <row r="44" spans="1:10">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="3"/>
       <c r="G44" s="9">
         <v>24</v>
@@ -1539,7 +1541,7 @@
     <row r="45" spans="1:10">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="3"/>
       <c r="G45" s="9">
         <v>25</v>
@@ -1551,7 +1553,7 @@
     <row r="46" spans="1:10">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="3"/>
       <c r="G46" s="9">
         <v>26</v>
@@ -1563,7 +1565,7 @@
     <row r="47" spans="1:10">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="3"/>
       <c r="G47" s="9">
         <v>27</v>
@@ -1575,7 +1577,7 @@
     <row r="48" spans="1:10">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="3"/>
       <c r="G48" s="9">
         <v>28</v>
@@ -1587,7 +1589,7 @@
     <row r="49" spans="1:8">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="3"/>
       <c r="G49" s="9">
         <v>29</v>
@@ -1600,6 +1602,7 @@
       <c r="A50" t="s">
         <v>76</v>
       </c>
+      <c r="C50" s="19"/>
       <c r="G50" s="9">
         <v>30</v>
       </c>
@@ -1608,6 +1611,7 @@
       </c>
     </row>
     <row r="51" spans="1:8">
+      <c r="C51" s="19"/>
       <c r="G51" s="9">
         <v>31</v>
       </c>
@@ -1615,9 +1619,71 @@
         <v>37</v>
       </c>
     </row>
+    <row r="52" spans="1:8">
+      <c r="C52" s="19"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="C53" s="19"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="C54" s="19"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="C55" s="19"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="C56" s="19"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="C57" s="19"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="C58" s="19"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="C59" s="19"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="C60" s="19"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="C61" s="19"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="C62" s="19"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="C63" s="19"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="C64" s="19"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="19"/>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="19"/>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" s="19"/>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="19"/>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="19"/>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" s="19"/>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71" s="19"/>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
edited template last row
</commit_message>
<xml_diff>
--- a/input/rds_template.xlsx
+++ b/input/rds_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1640" windowWidth="23320" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="2820" yWindow="360" windowWidth="23320" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -484,7 +486,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -526,6 +528,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -567,6 +570,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -899,7 +903,7 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A50" sqref="A50:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1599,10 +1603,10 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="19"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="3"/>
       <c r="G50" s="9">
         <v>30</v>
       </c>
@@ -1611,6 +1615,9 @@
       </c>
     </row>
     <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
       <c r="C51" s="19"/>
       <c r="G51" s="9">
         <v>31</v>
@@ -1684,6 +1691,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
lots of fixes inc rt2msg addition and times commas
</commit_message>
<xml_diff>
--- a/input/rds_template.xlsx
+++ b/input/rds_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="360" windowWidth="23320" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="2700" yWindow="0" windowWidth="23760" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>SHOW</t>
   </si>
@@ -33,12 +33,6 @@
     <t>22:02,23:02</t>
   </si>
   <si>
-    <t>RDS PTY CODE</t>
-  </si>
-  <si>
-    <t>RDS PROGRAMME TYPE</t>
-  </si>
-  <si>
     <t>No programme type defined</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Drama</t>
   </si>
   <si>
-    <t>Culture</t>
-  </si>
-  <si>
     <t>Science</t>
   </si>
   <si>
@@ -90,18 +81,12 @@
     <t>Other Music</t>
   </si>
   <si>
-    <t>Weather</t>
-  </si>
-  <si>
     <t>Finance</t>
   </si>
   <si>
     <t>Children's Programmes</t>
   </si>
   <si>
-    <t>Social Affairs</t>
-  </si>
-  <si>
     <t>Religion</t>
   </si>
   <si>
@@ -147,84 +132,93 @@
     <t>19:02</t>
   </si>
   <si>
-    <t>24:00</t>
-  </si>
-  <si>
     <t>DAYS</t>
   </si>
   <si>
+    <t>12:02</t>
+  </si>
+  <si>
+    <t>13:02,14:02,15:02</t>
+  </si>
+  <si>
+    <t>16:02,17:02,18:02</t>
+  </si>
+  <si>
+    <t>20:02,21:02,22:02,23:02</t>
+  </si>
+  <si>
+    <t>1=Monday</t>
+  </si>
+  <si>
+    <t>2=Tuesday</t>
+  </si>
+  <si>
+    <t>3=Wednesday</t>
+  </si>
+  <si>
+    <t>4=Thursday</t>
+  </si>
+  <si>
+    <t>5=Friday</t>
+  </si>
+  <si>
+    <t>6=Saturday</t>
+  </si>
+  <si>
+    <t>7=Sunday</t>
+  </si>
+  <si>
+    <t>GENRE CODES:</t>
+  </si>
+  <si>
+    <t>Days Codes:</t>
+  </si>
+  <si>
+    <t>Show Name:</t>
+  </si>
+  <si>
+    <t>Times:</t>
+  </si>
+  <si>
+    <t>This is the time the RDS display will switch to this message. Mostly 02 past the hour to account for the news at 00.</t>
+  </si>
+  <si>
+    <t>TEMPLATE GUIDE</t>
+  </si>
+  <si>
+    <t>Ensure the format matches other examples with no spaces (e.g 12:02,13:02)</t>
+  </si>
+  <si>
+    <t>06:02,07:02,08:02</t>
+  </si>
+  <si>
+    <t>General:</t>
+  </si>
+  <si>
+    <t>Custom Codes:</t>
+  </si>
+  <si>
+    <t>XX:00</t>
+  </si>
+  <si>
+    <t>I think there is a limit on RDS pro to 48 show entries (row 49 is the last one!). Entries show until they are set to change by another message.</t>
+  </si>
+  <si>
+    <t>LAST ENTRY!! (row 49)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX:00 means every top of the hour, XX:33 means every 33 mins past the hour etc…. (useful for the news) </t>
+  </si>
+  <si>
+    <t>The Breakfast Show</t>
+  </si>
+  <si>
+    <t>Mid Morning Show</t>
+  </si>
+  <si>
     <t>09:02,10:01,11:02</t>
   </si>
   <si>
-    <t>12:02</t>
-  </si>
-  <si>
-    <t>13:02,14:02,15:02</t>
-  </si>
-  <si>
-    <t>16:02,17:02,18:02</t>
-  </si>
-  <si>
-    <t>20:02,21:02,22:02,23:02</t>
-  </si>
-  <si>
-    <t>1=Monday</t>
-  </si>
-  <si>
-    <t>2=Tuesday</t>
-  </si>
-  <si>
-    <t>3=Wednesday</t>
-  </si>
-  <si>
-    <t>4=Thursday</t>
-  </si>
-  <si>
-    <t>5=Friday</t>
-  </si>
-  <si>
-    <t>6=Saturday</t>
-  </si>
-  <si>
-    <t>7=Sunday</t>
-  </si>
-  <si>
-    <t>GENRE CODES:</t>
-  </si>
-  <si>
-    <t>Days Codes:</t>
-  </si>
-  <si>
-    <t>Show Name:</t>
-  </si>
-  <si>
-    <t>Times:</t>
-  </si>
-  <si>
-    <t>This is the time the RDS display will switch to this message. Mostly 02 past the hour to account for the news at 00.</t>
-  </si>
-  <si>
-    <t>TEMPLATE GUIDE</t>
-  </si>
-  <si>
-    <t>Ensure the format matches other examples with no spaces (e.g 12:02,13:02)</t>
-  </si>
-  <si>
-    <t>06:02,07:02,08:02</t>
-  </si>
-  <si>
-    <t>There is a character limit, not sure exactly what it is at the moment but I know 54 characters is too long.</t>
-  </si>
-  <si>
-    <t>General:</t>
-  </si>
-  <si>
-    <t>The Breakfast Show</t>
-  </si>
-  <si>
-    <t>Mid Morning Show</t>
-  </si>
-  <si>
     <t>Lunchtime Show</t>
   </si>
   <si>
@@ -243,23 +237,32 @@
     <t>Late Night Tuesday</t>
   </si>
   <si>
+    <t>A Wednesday Show</t>
+  </si>
+  <si>
     <t>Late Night Thursday</t>
   </si>
   <si>
-    <t>A Wednesday Show</t>
-  </si>
-  <si>
-    <t>The line above is the last entry</t>
-  </si>
-  <si>
-    <t>I think there is a limit on RDS pro to 48 show entries. Entries show until they are set to change by another message.</t>
+    <t>A really long show name that needs to be a message</t>
+  </si>
+  <si>
+    <t>13:30</t>
+  </si>
+  <si>
+    <t>A super long show name that is way longer than 64 characters and so will be truncated</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>There is a character limit of 64. If the showname is longer, it will get truncated to 61 characters with "..." at the end.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -315,8 +318,23 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,8 +347,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -360,6 +390,17 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -367,7 +408,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,21 +494,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,14 +530,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -529,6 +585,11 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -571,10 +632,23 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -900,16 +974,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:D50"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="121.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -919,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -930,764 +1006,1153 @@
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3">
         <v>12345</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>63</v>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>77</v>
+      <c r="G2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3">
         <v>12345</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>44</v>
+      <c r="C3" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D3" s="3">
         <v>12</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3">
         <v>12345</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>45</v>
+      <c r="C4" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D4" s="3">
         <v>9</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>64</v>
+      <c r="G4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3">
         <v>12345</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>46</v>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D5" s="3">
         <v>12</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3">
         <v>12345</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>47</v>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>60</v>
+      <c r="G6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>41</v>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="3">
         <v>23</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>62</v>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
+      <c r="C8" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D8" s="3">
         <v>9</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D9" s="3">
         <v>9</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D10" s="3">
         <v>10</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="8" t="s">
         <v>50</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="3">
         <v>9</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5" t="s">
-        <v>51</v>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3">
         <v>1234567</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>42</v>
+      <c r="C12" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5" t="s">
-        <v>52</v>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="16">
-        <v>1234567</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="16">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>53</v>
+      <c r="A13" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="23">
+        <v>34</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="23">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
-        <v>54</v>
+      <c r="A14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="3"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="18"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="3"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5" t="s">
-        <v>55</v>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="3"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="17" t="s">
+        <v>48</v>
+      </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="3"/>
-      <c r="G17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="5"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="3"/>
-      <c r="G18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="G18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="7"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="3"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="15"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
       <c r="G20" s="9">
         <v>0</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="3"/>
       <c r="G21" s="9">
         <v>1</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="3"/>
       <c r="G22" s="9">
         <v>2</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="3"/>
       <c r="G23" s="9">
         <v>3</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="3"/>
       <c r="G24" s="9">
         <v>4</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="3"/>
       <c r="G25" s="9">
         <v>5</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="3"/>
       <c r="G26" s="9">
         <v>6</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="3"/>
       <c r="G27" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="3"/>
       <c r="G28" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="3"/>
       <c r="G29" s="9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="15"/>
       <c r="G30" s="9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="15"/>
       <c r="G31" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="3"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="15"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="3"/>
       <c r="G32" s="9">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:8">
       <c r="A33" s="3"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="15"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="3"/>
       <c r="G33" s="9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="3"/>
       <c r="G34" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" s="4"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="4"/>
       <c r="G35" s="9">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="3"/>
       <c r="G36" s="9">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="3"/>
       <c r="G37" s="9">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="3"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="15"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3"/>
       <c r="G38" s="9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
+      <c r="C39" s="5"/>
       <c r="D39" s="3"/>
       <c r="G39" s="9">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
+      <c r="C40" s="5"/>
       <c r="D40" s="3"/>
       <c r="G40" s="9">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
+      <c r="C41" s="5"/>
       <c r="D41" s="3"/>
       <c r="G41" s="9">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="3"/>
       <c r="G42" s="9">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="18"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="3"/>
       <c r="G43" s="9">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="18"/>
+      <c r="C44" s="21"/>
       <c r="D44" s="3"/>
       <c r="G44" s="9">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="18"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="3"/>
       <c r="G45" s="9">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="18"/>
+      <c r="C46" s="21"/>
       <c r="D46" s="3"/>
       <c r="G46" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="18"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="3"/>
       <c r="G47" s="9">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="18"/>
+      <c r="C48" s="21"/>
       <c r="D48" s="3"/>
       <c r="G48" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="18"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="3"/>
-      <c r="G49" s="9">
-        <v>29</v>
-      </c>
-      <c r="H49" s="10" t="s">
+      <c r="E49" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="C50" s="16"/>
+      <c r="G50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="19"/>
+      <c r="G51" s="9">
+        <v>32</v>
+      </c>
+      <c r="H51" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="3"/>
-      <c r="G50" s="9">
-        <v>30</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="19"/>
-      <c r="G51" s="9">
-        <v>31</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="52" spans="1:8">
-      <c r="C52" s="19"/>
+      <c r="C52" s="16"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="C53" s="19"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="C54" s="19"/>
+      <c r="C54" s="16"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="C55" s="19"/>
+      <c r="C55" s="16"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="C56" s="19"/>
+      <c r="C56" s="16"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="C57" s="19"/>
+      <c r="C57" s="16"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="C58" s="19"/>
+      <c r="C58" s="16"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="C59" s="19"/>
+      <c r="C59" s="16"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="C60" s="19"/>
+      <c r="C60" s="16"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="C61" s="19"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="C62" s="19"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="C63" s="19"/>
+      <c r="C63" s="16"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="C64" s="19"/>
+      <c r="C64" s="16"/>
     </row>
     <row r="65" spans="3:3">
-      <c r="C65" s="19"/>
+      <c r="C65" s="16"/>
     </row>
     <row r="66" spans="3:3">
-      <c r="C66" s="19"/>
+      <c r="C66" s="16"/>
     </row>
     <row r="67" spans="3:3">
-      <c r="C67" s="19"/>
+      <c r="C67" s="16"/>
     </row>
     <row r="68" spans="3:3">
-      <c r="C68" s="19"/>
+      <c r="C68" s="16"/>
     </row>
     <row r="69" spans="3:3">
-      <c r="C69" s="19"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="70" spans="3:3">
-      <c r="C70" s="19"/>
+      <c r="C70" s="16"/>
     </row>
     <row r="71" spans="3:3">
-      <c r="C71" s="19"/>
+      <c r="C71" s="16"/>
     </row>
     <row r="72" spans="3:3">
-      <c r="C72" s="19"/>
+      <c r="C72" s="16"/>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" s="16"/>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" s="16"/>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" s="16"/>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="16"/>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" s="16"/>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" s="16"/>
+    </row>
+    <row r="79" spans="3:3">
+      <c r="C79" s="16"/>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" s="16"/>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="16"/>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="16"/>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" s="16"/>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" s="16"/>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" s="16"/>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="16"/>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" s="16"/>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="16"/>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" s="16"/>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90" s="16"/>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="16"/>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" s="16"/>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="16"/>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" s="16"/>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95" s="16"/>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96" s="16"/>
+    </row>
+    <row r="97" spans="3:3">
+      <c r="C97" s="16"/>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="16"/>
+    </row>
+    <row r="99" spans="3:3">
+      <c r="C99" s="16"/>
+    </row>
+    <row r="100" spans="3:3">
+      <c r="C100" s="16"/>
+    </row>
+    <row r="101" spans="3:3">
+      <c r="C101" s="16"/>
+    </row>
+    <row r="102" spans="3:3">
+      <c r="C102" s="16"/>
+    </row>
+    <row r="103" spans="3:3">
+      <c r="C103" s="16"/>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104" s="16"/>
+    </row>
+    <row r="105" spans="3:3">
+      <c r="C105" s="16"/>
+    </row>
+    <row r="106" spans="3:3">
+      <c r="C106" s="16"/>
+    </row>
+    <row r="107" spans="3:3">
+      <c r="C107" s="16"/>
+    </row>
+    <row r="108" spans="3:3">
+      <c r="C108" s="16"/>
+    </row>
+    <row r="109" spans="3:3">
+      <c r="C109" s="16"/>
+    </row>
+    <row r="110" spans="3:3">
+      <c r="C110" s="16"/>
+    </row>
+    <row r="111" spans="3:3">
+      <c r="C111" s="16"/>
+    </row>
+    <row r="112" spans="3:3">
+      <c r="C112" s="16"/>
+    </row>
+    <row r="113" spans="3:3">
+      <c r="C113" s="16"/>
+    </row>
+    <row r="114" spans="3:3">
+      <c r="C114" s="16"/>
+    </row>
+    <row r="115" spans="3:3">
+      <c r="C115" s="16"/>
+    </row>
+    <row r="116" spans="3:3">
+      <c r="C116" s="16"/>
+    </row>
+    <row r="117" spans="3:3">
+      <c r="C117" s="16"/>
+    </row>
+    <row r="118" spans="3:3">
+      <c r="C118" s="16"/>
+    </row>
+    <row r="119" spans="3:3">
+      <c r="C119" s="16"/>
+    </row>
+    <row r="120" spans="3:3">
+      <c r="C120" s="16"/>
+    </row>
+    <row r="121" spans="3:3">
+      <c r="C121" s="16"/>
+    </row>
+    <row r="122" spans="3:3">
+      <c r="C122" s="16"/>
+    </row>
+    <row r="123" spans="3:3">
+      <c r="C123" s="16"/>
+    </row>
+    <row r="124" spans="3:3">
+      <c r="C124" s="16"/>
+    </row>
+    <row r="125" spans="3:3">
+      <c r="C125" s="16"/>
+    </row>
+    <row r="126" spans="3:3">
+      <c r="C126" s="16"/>
+    </row>
+    <row r="127" spans="3:3">
+      <c r="C127" s="16"/>
+    </row>
+    <row r="128" spans="3:3">
+      <c r="C128" s="16"/>
+    </row>
+    <row r="129" spans="3:3">
+      <c r="C129" s="16"/>
+    </row>
+    <row r="130" spans="3:3">
+      <c r="C130" s="16"/>
+    </row>
+    <row r="131" spans="3:3">
+      <c r="C131" s="16"/>
+    </row>
+    <row r="132" spans="3:3">
+      <c r="C132" s="16"/>
+    </row>
+    <row r="133" spans="3:3">
+      <c r="C133" s="16"/>
+    </row>
+    <row r="134" spans="3:3">
+      <c r="C134" s="16"/>
+    </row>
+    <row r="135" spans="3:3">
+      <c r="C135" s="16"/>
+    </row>
+    <row r="136" spans="3:3">
+      <c r="C136" s="16"/>
+    </row>
+    <row r="137" spans="3:3">
+      <c r="C137" s="16"/>
+    </row>
+    <row r="138" spans="3:3">
+      <c r="C138" s="16"/>
+    </row>
+    <row r="139" spans="3:3">
+      <c r="C139" s="16"/>
+    </row>
+    <row r="140" spans="3:3">
+      <c r="C140" s="16"/>
+    </row>
+    <row r="141" spans="3:3">
+      <c r="C141" s="16"/>
+    </row>
+    <row r="142" spans="3:3">
+      <c r="C142" s="16"/>
+    </row>
+    <row r="143" spans="3:3">
+      <c r="C143" s="16"/>
+    </row>
+    <row r="144" spans="3:3">
+      <c r="C144" s="16"/>
+    </row>
+    <row r="145" spans="3:3">
+      <c r="C145" s="16"/>
+    </row>
+    <row r="146" spans="3:3">
+      <c r="C146" s="16"/>
+    </row>
+    <row r="147" spans="3:3">
+      <c r="C147" s="16"/>
+    </row>
+    <row r="148" spans="3:3">
+      <c r="C148" s="16"/>
+    </row>
+    <row r="149" spans="3:3">
+      <c r="C149" s="16"/>
+    </row>
+    <row r="150" spans="3:3">
+      <c r="C150" s="16"/>
+    </row>
+    <row r="151" spans="3:3">
+      <c r="C151" s="16"/>
+    </row>
+    <row r="152" spans="3:3">
+      <c r="C152" s="16"/>
+    </row>
+    <row r="153" spans="3:3">
+      <c r="C153" s="16"/>
+    </row>
+    <row r="154" spans="3:3">
+      <c r="C154" s="16"/>
+    </row>
+    <row r="155" spans="3:3">
+      <c r="C155" s="16"/>
+    </row>
+    <row r="156" spans="3:3">
+      <c r="C156" s="16"/>
+    </row>
+    <row r="157" spans="3:3">
+      <c r="C157" s="16"/>
+    </row>
+    <row r="158" spans="3:3">
+      <c r="C158" s="16"/>
+    </row>
+    <row r="159" spans="3:3">
+      <c r="C159" s="16"/>
+    </row>
+    <row r="160" spans="3:3">
+      <c r="C160" s="16"/>
+    </row>
+    <row r="161" spans="3:3">
+      <c r="C161" s="16"/>
+    </row>
+    <row r="162" spans="3:3">
+      <c r="C162" s="16"/>
+    </row>
+    <row r="163" spans="3:3">
+      <c r="C163" s="16"/>
+    </row>
+    <row r="164" spans="3:3">
+      <c r="C164" s="16"/>
+    </row>
+    <row r="165" spans="3:3">
+      <c r="C165" s="16"/>
+    </row>
+    <row r="166" spans="3:3">
+      <c r="C166" s="16"/>
+    </row>
+    <row r="167" spans="3:3">
+      <c r="C167" s="16"/>
+    </row>
+    <row r="168" spans="3:3">
+      <c r="C168" s="16"/>
+    </row>
+    <row r="169" spans="3:3">
+      <c r="C169" s="16"/>
+    </row>
+    <row r="170" spans="3:3">
+      <c r="C170" s="16"/>
+    </row>
+    <row r="171" spans="3:3">
+      <c r="C171" s="16"/>
+    </row>
+    <row r="172" spans="3:3">
+      <c r="C172" s="16"/>
+    </row>
+    <row r="173" spans="3:3">
+      <c r="C173" s="16"/>
+    </row>
+    <row r="174" spans="3:3">
+      <c r="C174" s="16"/>
+    </row>
+    <row r="175" spans="3:3">
+      <c r="C175" s="16"/>
+    </row>
+    <row r="176" spans="3:3">
+      <c r="C176" s="16"/>
+    </row>
+    <row r="177" spans="3:3">
+      <c r="C177" s="16"/>
+    </row>
+    <row r="178" spans="3:3">
+      <c r="C178" s="16"/>
+    </row>
+    <row r="179" spans="3:3">
+      <c r="C179" s="16"/>
+    </row>
+    <row r="180" spans="3:3">
+      <c r="C180" s="16"/>
+    </row>
+    <row r="181" spans="3:3">
+      <c r="C181" s="16"/>
+    </row>
+    <row r="182" spans="3:3">
+      <c r="C182" s="16"/>
+    </row>
+    <row r="183" spans="3:3">
+      <c r="C183" s="16"/>
+    </row>
+    <row r="184" spans="3:3">
+      <c r="C184" s="16"/>
+    </row>
+    <row r="185" spans="3:3">
+      <c r="C185" s="16"/>
+    </row>
+    <row r="186" spans="3:3">
+      <c r="C186" s="16"/>
+    </row>
+    <row r="187" spans="3:3">
+      <c r="C187" s="16"/>
+    </row>
+    <row r="188" spans="3:3">
+      <c r="C188" s="16"/>
+    </row>
+    <row r="189" spans="3:3">
+      <c r="C189" s="16"/>
+    </row>
+    <row r="190" spans="3:3">
+      <c r="C190" s="16"/>
+    </row>
+    <row r="191" spans="3:3">
+      <c r="C191" s="16"/>
+    </row>
+    <row r="192" spans="3:3">
+      <c r="C192" s="16"/>
+    </row>
+    <row r="193" spans="3:3">
+      <c r="C193" s="16"/>
+    </row>
+    <row r="194" spans="3:3">
+      <c r="C194" s="16"/>
+    </row>
+    <row r="195" spans="3:3">
+      <c r="C195" s="16"/>
+    </row>
+    <row r="196" spans="3:3">
+      <c r="C196" s="16"/>
+    </row>
+    <row r="197" spans="3:3">
+      <c r="C197" s="16"/>
+    </row>
+    <row r="198" spans="3:3">
+      <c r="C198" s="16"/>
+    </row>
+    <row r="199" spans="3:3">
+      <c r="C199" s="16"/>
+    </row>
+    <row r="200" spans="3:3">
+      <c r="C200" s="16"/>
+    </row>
+    <row r="201" spans="3:3">
+      <c r="C201" s="16"/>
+    </row>
+    <row r="202" spans="3:3">
+      <c r="C202" s="16"/>
+    </row>
+    <row r="203" spans="3:3">
+      <c r="C203" s="16"/>
+    </row>
+    <row r="204" spans="3:3">
+      <c r="C204" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>